<commit_message>
Archiving master file works; no error checking yet.
</commit_message>
<xml_diff>
--- a/blank_excel_files_templates/master_fantasy_book_list_BLANK.xlsx
+++ b/blank_excel_files_templates/master_fantasy_book_list_BLANK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\p\fantasy_books_workspace\fantasy_books\blank_excel_files_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1F62C-B50D-4BFB-BAC6-CB53CDF4DCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D31BD2-4618-4AA4-99ED-BB024E925F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="2955" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master List" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="GLS" localSheetId="0">'Master List'!$A$1:$AV$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -581,8 +581,8 @@
     <col min="41" max="48" width="9.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="37.140625" style="1" customWidth="1"/>
     <col min="50" max="50" width="18.140625" style="1" customWidth="1"/>
-    <col min="51" max="71" width="9.140625" style="1" customWidth="1"/>
-    <col min="72" max="16384" width="9.140625" style="1"/>
+    <col min="51" max="58" width="9.140625" style="1" customWidth="1"/>
+    <col min="59" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -739,6 +739,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>